<commit_message>
Added sprites and The Eye
</commit_message>
<xml_diff>
--- a/GameRules.xlsx
+++ b/GameRules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffithcollege628-my.sharepoint.com/personal/evandro_gomezquintino_student_griffith_ie/Documents/Griffith College/Project4th/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffithcollege628-my.sharepoint.com/personal/evandro_gomezquintino_student_griffith_ie/Documents/Griffith College/Project4th/LOTR_Tactics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{C8547F04-AF29-4A80-845D-8FBB07732555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F8929D8-63B6-4798-97BC-883EF7745849}"/>
@@ -357,14 +357,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -744,8 +744,8 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
@@ -832,7 +832,7 @@
   <dimension ref="B2:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -841,32 +841,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="2:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="S3" s="16" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="S3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
@@ -1071,45 +1071,45 @@
       <c r="R24" s="11"/>
     </row>
     <row r="25" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>35</v>
       </c>
       <c r="F25" s="11"/>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I25" s="17" t="s">
         <v>39</v>
       </c>
       <c r="R25" s="11"/>
     </row>
     <row r="26" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="16" t="s">
         <v>30</v>
       </c>
       <c r="F26" s="11"/>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="16" t="s">
         <v>38</v>
       </c>
       <c r="R26" s="11" t="s">
@@ -1117,23 +1117,23 @@
       </c>
     </row>
     <row r="27" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="11"/>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="16" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding tons of updates. Added mechanics, removed unecessary code, updated documentation.
</commit_message>
<xml_diff>
--- a/GameRules.xlsx
+++ b/GameRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffithcollege628-my.sharepoint.com/personal/evandro_gomezquintino_student_griffith_ie/Documents/Griffith College/Project4th/LOTR_Tactics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{C8547F04-AF29-4A80-845D-8FBB07732555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F8929D8-63B6-4798-97BC-883EF7745849}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{C8547F04-AF29-4A80-845D-8FBB07732555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{79CB9FFF-67AE-4411-A760-437D721CDE1E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{550C3DAD-91DF-4502-BC50-3CC89E8E81C9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{550C3DAD-91DF-4502-BC50-3CC89E8E81C9}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Rules" sheetId="1" r:id="rId1"/>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4746EBAF-FC61-48A2-A459-E06E203930D2}">
   <dimension ref="B2:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>